<commit_message>
Screenshots of the results graphs
</commit_message>
<xml_diff>
--- a/megaavr/extras/testCases/periodicNoise/results.xlsx
+++ b/megaavr/extras/testCases/periodicNoise/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Desktop\School\22-23 Spring\SER 402\DxCore\megaavr\extras\testCases\periodicNoise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5786F5EB-ACD2-42FA-AF70-006A4A1D61BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B0309E-DB4F-4638-ADD0-70803DF80164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,15 +112,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1046,11 +1043,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Voltage Reading /</a:t>
+              <a:t>Voltage Reading with</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Num Samples with 4 samples accumulated</a:t>
+              <a:t> noise and 4 samples accumulated</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1876,7 +1873,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Voltage Reading / Num Samples with 16 samples accumulated</a:t>
+              <a:t>Voltage Reading with noise and</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>16 samples accumulated</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2594,44 +2599,11 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="578716944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -2778,7 +2750,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Voltage Reading / Num Samples with 64 samples accumulated</a:t>
+              <a:t>Voltage Reading with noise and 64 samples accumulated</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3496,44 +3468,11 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="578716944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -3565,7 +3504,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -6297,8 +6236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6325,15 +6264,15 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <f>AVERAGE(B12:B221)</f>
         <v>1559.2380952380952</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <f t="shared" ref="C2:D2" si="0">AVERAGE(C12:C221)</f>
         <v>6231.3857142857141</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <f t="shared" si="0"/>
         <v>24923.795238095237</v>
       </c>
@@ -6342,15 +6281,15 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <f>MIN(B12:B221)</f>
         <v>1525</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <f>MIN(C12:C221)</f>
         <v>6160</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <f>MIN(D12:D221)</f>
         <v>24889</v>
       </c>
@@ -6359,15 +6298,15 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <f>MAX(B12:B221)</f>
         <v>1586</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <f t="shared" ref="C4:D4" si="1">MAX(C12:C221)</f>
         <v>6283</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <f t="shared" si="1"/>
         <v>24960</v>
       </c>
@@ -6376,37 +6315,37 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <f>B4-B3</f>
         <v>61</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <f t="shared" ref="C5:D5" si="2">C4-C3</f>
         <v>123</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <f>B2/B1</f>
         <v>389.8095238095238</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <f>C2/C1</f>
         <v>389.46160714285713</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <f>D2/D1</f>
         <v>389.43430059523808</v>
       </c>
@@ -6415,15 +6354,15 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <f>B3/B1</f>
         <v>381.25</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <f t="shared" ref="C8:D8" si="3">C3/C1</f>
         <v>385</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <f t="shared" si="3"/>
         <v>388.890625</v>
       </c>
@@ -6432,15 +6371,15 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <f>B4/B1</f>
         <v>396.5</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <f t="shared" ref="C9:D9" si="4">C4/C1</f>
         <v>392.6875</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <f t="shared" si="4"/>
         <v>390</v>
       </c>
@@ -6449,15 +6388,15 @@
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <f>B5/B1</f>
         <v>15.25</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <f t="shared" ref="C10:D10" si="5">C5/C1</f>
         <v>7.6875</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
         <f t="shared" si="5"/>
         <v>1.109375</v>
       </c>

</xml_diff>